<commit_message>
Implement recommendations (review 2)
</commit_message>
<xml_diff>
--- a/data/recipe_data.xlsx
+++ b/data/recipe_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\foodgram-project-react\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA16826-283F-4743-A5B0-C6E41B82E2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC88951B-501C-4842-A325-D71CED346721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="160" windowWidth="20710" windowHeight="11590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>ivan</t>
   </si>
   <si>
-    <t>ivan@example.com</t>
-  </si>
-  <si>
     <t>secret-code+1</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>petr</t>
   </si>
   <si>
-    <t>petr@example.com</t>
-  </si>
-  <si>
     <t>secret-code+2</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>fedor</t>
   </si>
   <si>
-    <t>fedor@example.com</t>
-  </si>
-  <si>
     <t>secret-code+3</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>elena</t>
   </si>
   <si>
-    <t>elena@example.com</t>
-  </si>
-  <si>
     <t>secret-code+4</t>
   </si>
   <si>
@@ -118,9 +106,6 @@
     <t>anastasia</t>
   </si>
   <si>
-    <t>anastasia@example.com</t>
-  </si>
-  <si>
     <t>secret-code+5</t>
   </si>
   <si>
@@ -133,9 +118,6 @@
     <t>kristina</t>
   </si>
   <si>
-    <t>kristina@example.com</t>
-  </si>
-  <si>
     <t>secret-code+6</t>
   </si>
   <si>
@@ -146,9 +128,6 @@
   </si>
   <si>
     <t>alexandra</t>
-  </si>
-  <si>
-    <t>alexandra@example.com</t>
   </si>
   <si>
     <t>secret-code+7</t>
@@ -671,6 +650,27 @@
   </si>
   <si>
     <t>recipes/images/1.jpg</t>
+  </si>
+  <si>
+    <t>abcd@example.com</t>
+  </si>
+  <si>
+    <t>efgh@example.com</t>
+  </si>
+  <si>
+    <t>ijkl@example.com</t>
+  </si>
+  <si>
+    <t>mnop@example.com</t>
+  </si>
+  <si>
+    <t>qrst@example.com</t>
+  </si>
+  <si>
+    <t>uvwx@example.com</t>
+  </si>
+  <si>
+    <t>yzab@example.com</t>
   </si>
 </sst>
 </file>
@@ -1022,112 +1022,112 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1145,68 +1145,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1227,30 +1227,30 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E2">
         <v>180</v>
@@ -1258,16 +1258,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E3">
         <v>70</v>
@@ -1275,16 +1275,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -1292,16 +1292,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1309,16 +1309,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E6">
         <v>45</v>
@@ -1326,16 +1326,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -1343,16 +1343,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -1360,16 +1360,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E9">
         <v>20</v>
@@ -1377,16 +1377,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>60</v>
@@ -1394,16 +1394,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E11">
         <v>40</v>
@@ -1411,16 +1411,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -1431,13 +1431,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E13">
         <v>50</v>
@@ -1448,13 +1448,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E14">
         <v>60</v>
@@ -1465,13 +1465,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E15">
         <v>150</v>
@@ -1482,13 +1482,13 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -1499,13 +1499,13 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E17">
         <v>40</v>
@@ -1516,13 +1516,13 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E18">
         <v>35</v>
@@ -1533,13 +1533,13 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E19">
         <v>40</v>
@@ -1563,16 +1563,16 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1580,16 +1580,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D2">
         <v>220</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1597,16 +1597,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>400</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1614,16 +1614,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
       </c>
       <c r="D4">
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1631,16 +1631,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D5">
         <v>300</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1648,16 +1648,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D6">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1665,16 +1665,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1682,16 +1682,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D8">
         <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1699,16 +1699,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D9">
         <v>700</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1716,16 +1716,16 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D10">
         <v>180</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1733,16 +1733,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D11">
         <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1750,16 +1750,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D12">
         <v>3000</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1767,16 +1767,16 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>1000</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1784,16 +1784,16 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D14">
         <v>336</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1801,16 +1801,16 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D15">
         <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1818,16 +1818,16 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1835,16 +1835,16 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D17">
         <v>420</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1852,16 +1852,16 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D18">
         <v>150</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1869,16 +1869,16 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D19">
         <v>140</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1886,16 +1886,16 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1903,16 +1903,16 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D21">
         <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1920,16 +1920,16 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D22">
         <v>180</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1937,16 +1937,16 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1954,16 +1954,16 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D24">
         <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1971,16 +1971,16 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D25">
         <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1988,16 +1988,16 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D26">
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -2005,16 +2005,16 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -2022,16 +2022,16 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D28">
         <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -2039,16 +2039,16 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D29">
         <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -2056,16 +2056,16 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D30">
         <v>150</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -2073,16 +2073,16 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D31">
         <v>200</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -2090,16 +2090,16 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D32">
         <v>100</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -2107,16 +2107,16 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -2124,16 +2124,16 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D34">
         <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -2141,16 +2141,16 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D35">
         <v>200</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -2158,16 +2158,16 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D36">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -2175,16 +2175,16 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D37">
         <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -2192,16 +2192,16 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D38">
         <v>1200</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -2209,16 +2209,16 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D39">
         <v>100</v>
       </c>
       <c r="E39" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -2226,16 +2226,16 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -2243,16 +2243,16 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -2260,16 +2260,16 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -2277,16 +2277,16 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D43">
         <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -2294,16 +2294,16 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -2311,16 +2311,16 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -2328,16 +2328,16 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D46">
         <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -2345,16 +2345,16 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D47">
         <v>60</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -2362,16 +2362,16 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D48">
         <v>500</v>
       </c>
       <c r="E48" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -2379,16 +2379,16 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D49">
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -2396,16 +2396,16 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D50">
         <v>130</v>
       </c>
       <c r="E50" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -2413,16 +2413,16 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D51">
         <v>90</v>
       </c>
       <c r="E51" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -2430,1563 +2430,1563 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D52">
         <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D53">
         <v>500</v>
       </c>
       <c r="E53" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D55">
         <v>130</v>
       </c>
       <c r="E55" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D56">
         <v>30</v>
       </c>
       <c r="E56" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D57">
         <v>250</v>
       </c>
       <c r="E57" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D59">
         <v>40</v>
       </c>
       <c r="E59" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D60">
         <v>100</v>
       </c>
       <c r="E60" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D61">
         <v>500</v>
       </c>
       <c r="E61" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D62">
         <v>120</v>
       </c>
       <c r="E62" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D63">
         <v>40</v>
       </c>
       <c r="E63" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D64">
         <v>50</v>
       </c>
       <c r="E64" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D65">
         <v>44</v>
       </c>
       <c r="E65" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D66">
         <v>52</v>
       </c>
       <c r="E66" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D69">
         <v>150</v>
       </c>
       <c r="E69" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D71">
         <v>150</v>
       </c>
       <c r="E71" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D72">
         <v>6</v>
       </c>
       <c r="E72" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D73">
         <v>65</v>
       </c>
       <c r="E73" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D74">
         <v>200</v>
       </c>
       <c r="E74" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D75">
         <v>50</v>
       </c>
       <c r="E75" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D76">
         <v>195</v>
       </c>
       <c r="E76" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D77">
         <v>180</v>
       </c>
       <c r="E77" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C78" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D78">
         <v>50</v>
       </c>
       <c r="E78" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D79">
         <v>80</v>
       </c>
       <c r="E79" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D80">
         <v>25</v>
       </c>
       <c r="E80" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D81">
         <v>50</v>
       </c>
       <c r="E81" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C84" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D84">
         <v>400</v>
       </c>
       <c r="E84" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D85">
         <v>3</v>
       </c>
       <c r="E85" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C86" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D86">
         <v>150</v>
       </c>
       <c r="E86" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D87">
         <v>26</v>
       </c>
       <c r="E87" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C88" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D88">
         <v>195</v>
       </c>
       <c r="E88" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C89" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D89">
         <v>100</v>
       </c>
       <c r="E89" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C91" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C92" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D92">
         <v>600</v>
       </c>
       <c r="E92" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C93" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D93">
         <v>400</v>
       </c>
       <c r="E93" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C94" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D94">
         <v>250</v>
       </c>
       <c r="E94" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C95" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D95">
         <v>100</v>
       </c>
       <c r="E95" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C96" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D96">
         <v>6</v>
       </c>
       <c r="E96" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C97" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D97">
         <v>65</v>
       </c>
       <c r="E97" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C98" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D98">
         <v>20</v>
       </c>
       <c r="E98" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C99" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D99">
         <v>40</v>
       </c>
       <c r="E99" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B100" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C100" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D100">
         <v>4</v>
       </c>
       <c r="E100" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C101" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B102" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C102" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D102">
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B103" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C103" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D103">
         <v>220</v>
       </c>
       <c r="E103" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B104" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D104">
         <v>660</v>
       </c>
       <c r="E104" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C105" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D105">
         <v>500</v>
       </c>
       <c r="E105" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B106" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C106" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D106">
         <v>50</v>
       </c>
       <c r="E106" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C107" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D107">
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B108" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C108" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D108">
         <v>80</v>
       </c>
       <c r="E108" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B109" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C109" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D109">
         <v>160</v>
       </c>
       <c r="E109" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B110" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C110" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D110">
         <v>65</v>
       </c>
       <c r="E110" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C111" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D111">
         <v>2</v>
       </c>
       <c r="E111" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B112" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C112" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D112">
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B113" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C113" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D113">
         <v>200</v>
       </c>
       <c r="E113" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B114" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C114" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D114">
         <v>325</v>
       </c>
       <c r="E114" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C115" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D115">
         <v>150</v>
       </c>
       <c r="E115" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B116" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D116">
         <v>60</v>
       </c>
       <c r="E116" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B117" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C117" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D117">
         <v>100</v>
       </c>
       <c r="E117" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B118" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C118" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D118">
         <v>40</v>
       </c>
       <c r="E118" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B119" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C119" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D119">
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B120" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C120" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D120">
         <v>1</v>
       </c>
       <c r="E120" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B121" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C121" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D121">
         <v>1500</v>
       </c>
       <c r="E121" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B122" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C122" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D122">
         <v>500</v>
       </c>
       <c r="E122" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B123" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C123" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D123">
         <v>80</v>
       </c>
       <c r="E123" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B124" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C124" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D124">
         <v>30</v>
       </c>
       <c r="E124" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B125" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C125" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D125">
         <v>112</v>
       </c>
       <c r="E125" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B126" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C126" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D126">
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B127" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C127" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D127">
         <v>5</v>
       </c>
       <c r="E127" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B128" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C128" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D128">
         <v>1</v>
       </c>
       <c r="E128" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B129" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C129" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D129">
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B130" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C130" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D130">
         <v>400</v>
       </c>
       <c r="E130" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B131" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C131" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D131">
         <v>240</v>
       </c>
       <c r="E131" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B132" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C132" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D132">
         <v>300</v>
       </c>
       <c r="E132" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B133" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C133" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D133">
         <v>112</v>
       </c>
       <c r="E133" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B134" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C134" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D134">
         <v>100</v>
       </c>
       <c r="E134" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B135" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C135" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D135">
         <v>50</v>
       </c>
       <c r="E135" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B136" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C136" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D136">
         <v>1</v>
       </c>
       <c r="E136" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B137" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C137" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D137">
         <v>1</v>
       </c>
       <c r="E137" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B138" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C138" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D138">
         <v>50</v>
       </c>
       <c r="E138" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B139" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C139" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D139">
         <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B140" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C140" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D140">
         <v>1</v>
       </c>
       <c r="E140" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B141" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C141" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D141">
         <v>3</v>
       </c>
       <c r="E141" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B142" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C142" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D142">
         <v>100</v>
       </c>
       <c r="E142" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B143" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C143" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D143">
         <v>30</v>
       </c>
       <c r="E143" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -4007,10 +4007,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -4018,10 +4018,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -4029,10 +4029,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -4040,10 +4040,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -4051,10 +4051,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -4062,10 +4062,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -4073,10 +4073,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -4084,10 +4084,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -4095,10 +4095,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -4106,10 +4106,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -4117,164 +4117,164 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
         <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>